<commit_message>
update Scott and Alex's data
update Scott and Alex's data
</commit_message>
<xml_diff>
--- a/TheBiggestLoser.xlsx
+++ b/TheBiggestLoser.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Alex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +62,6 @@
   </si>
   <si>
     <t>Team L</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -104,7 +100,7 @@
       <name val="MV Boli"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,12 +137,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -175,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,9 +207,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -594,7 +581,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -614,8 +601,8 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>12</v>
+      <c r="B2" s="10">
+        <v>86.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -638,8 +625,8 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>12</v>
+      <c r="B5" s="10">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -656,7 +643,7 @@
       </c>
       <c r="B7" s="11">
         <f>SUM(B2:B6)</f>
-        <v>199</v>
+        <v>350.90000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -682,8 +669,8 @@
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>13</v>
+      <c r="B11" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>